<commit_message>
Updates code base and input data. Big commit.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -180,15 +180,14 @@
   </sheetPr>
   <dimension ref="A1:AF72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y8" activeCellId="0" sqref="Y8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N46" activeCellId="0" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6337,7 +6336,7 @@
         <v>1</v>
       </c>
       <c r="R57" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S57" s="2" t="n">
         <v>0</v>
@@ -6370,7 +6369,7 @@
       </c>
       <c r="AA57" s="3" t="n">
         <f aca="false">SUM(L57, R57)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB57" s="3" t="n">
         <f aca="false">SUM(N57:O57)</f>
@@ -6390,7 +6389,7 @@
       </c>
       <c r="AF57" s="3" t="n">
         <f aca="false">SUM(B57:U57)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Reworked compiling data. Adds inferential stats.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>offensive</t>
+  </si>
+  <si>
+    <t>defensive</t>
   </si>
 </sst>
 </file>
@@ -178,16 +184,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF72"/>
+  <dimension ref="A1:AH72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N46" activeCellId="0" sqref="N46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM8" activeCellId="0" sqref="AM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,6 +294,12 @@
       <c r="AF1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="AG1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -396,6 +409,14 @@
         <f aca="false">SUM(B2:U2)</f>
         <v>19</v>
       </c>
+      <c r="AG2" s="0" t="n">
+        <f aca="false">SUM(AA2:AE2)</f>
+        <v>9</v>
+      </c>
+      <c r="AH2" s="0" t="n">
+        <f aca="false">SUM(V2:Z2)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -505,6 +526,14 @@
         <f aca="false">SUM(B3:U3)</f>
         <v>20</v>
       </c>
+      <c r="AG3" s="0" t="n">
+        <f aca="false">SUM(AA3:AE3)</f>
+        <v>10</v>
+      </c>
+      <c r="AH3" s="0" t="n">
+        <f aca="false">SUM(V3:Z3)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -614,6 +643,14 @@
         <f aca="false">SUM(B4:U4)</f>
         <v>19</v>
       </c>
+      <c r="AG4" s="0" t="n">
+        <f aca="false">SUM(AA4:AE4)</f>
+        <v>10</v>
+      </c>
+      <c r="AH4" s="0" t="n">
+        <f aca="false">SUM(V4:Z4)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -723,6 +760,14 @@
         <f aca="false">SUM(B5:U5)</f>
         <v>20</v>
       </c>
+      <c r="AG5" s="0" t="n">
+        <f aca="false">SUM(AA5:AE5)</f>
+        <v>10</v>
+      </c>
+      <c r="AH5" s="0" t="n">
+        <f aca="false">SUM(V5:Z5)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -832,6 +877,14 @@
         <f aca="false">SUM(B6:U6)</f>
         <v>19</v>
       </c>
+      <c r="AG6" s="0" t="n">
+        <f aca="false">SUM(AA6:AE6)</f>
+        <v>10</v>
+      </c>
+      <c r="AH6" s="0" t="n">
+        <f aca="false">SUM(V6:Z6)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -941,6 +994,14 @@
         <f aca="false">SUM(B7:U7)</f>
         <v>19</v>
       </c>
+      <c r="AG7" s="0" t="n">
+        <f aca="false">SUM(AA7:AE7)</f>
+        <v>10</v>
+      </c>
+      <c r="AH7" s="0" t="n">
+        <f aca="false">SUM(V7:Z7)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -1050,6 +1111,14 @@
         <f aca="false">SUM(B8:U8)</f>
         <v>19</v>
       </c>
+      <c r="AG8" s="0" t="n">
+        <f aca="false">SUM(AA8:AE8)</f>
+        <v>10</v>
+      </c>
+      <c r="AH8" s="0" t="n">
+        <f aca="false">SUM(V8:Z8)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1159,6 +1228,14 @@
         <f aca="false">SUM(B9:U9)</f>
         <v>19</v>
       </c>
+      <c r="AG9" s="0" t="n">
+        <f aca="false">SUM(AA9:AE9)</f>
+        <v>10</v>
+      </c>
+      <c r="AH9" s="0" t="n">
+        <f aca="false">SUM(V9:Z9)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -1268,6 +1345,14 @@
         <f aca="false">SUM(B10:U10)</f>
         <v>19</v>
       </c>
+      <c r="AG10" s="0" t="n">
+        <f aca="false">SUM(AA10:AE10)</f>
+        <v>10</v>
+      </c>
+      <c r="AH10" s="0" t="n">
+        <f aca="false">SUM(V10:Z10)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1377,6 +1462,14 @@
         <f aca="false">SUM(B11:U11)</f>
         <v>18</v>
       </c>
+      <c r="AG11" s="0" t="n">
+        <f aca="false">SUM(AA11:AE11)</f>
+        <v>9</v>
+      </c>
+      <c r="AH11" s="0" t="n">
+        <f aca="false">SUM(V11:Z11)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1486,6 +1579,14 @@
         <f aca="false">SUM(B12:U12)</f>
         <v>19</v>
       </c>
+      <c r="AG12" s="0" t="n">
+        <f aca="false">SUM(AA12:AE12)</f>
+        <v>10</v>
+      </c>
+      <c r="AH12" s="0" t="n">
+        <f aca="false">SUM(V12:Z12)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -1595,6 +1696,14 @@
         <f aca="false">SUM(B13:U13)</f>
         <v>19</v>
       </c>
+      <c r="AG13" s="0" t="n">
+        <f aca="false">SUM(AA13:AE13)</f>
+        <v>10</v>
+      </c>
+      <c r="AH13" s="0" t="n">
+        <f aca="false">SUM(V13:Z13)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -1704,6 +1813,14 @@
         <f aca="false">SUM(B14:U14)</f>
         <v>18</v>
       </c>
+      <c r="AG14" s="0" t="n">
+        <f aca="false">SUM(AA14:AE14)</f>
+        <v>9</v>
+      </c>
+      <c r="AH14" s="0" t="n">
+        <f aca="false">SUM(V14:Z14)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1813,6 +1930,14 @@
         <f aca="false">SUM(B15:U15)</f>
         <v>18</v>
       </c>
+      <c r="AG15" s="0" t="n">
+        <f aca="false">SUM(AA15:AE15)</f>
+        <v>9</v>
+      </c>
+      <c r="AH15" s="0" t="n">
+        <f aca="false">SUM(V15:Z15)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1922,6 +2047,14 @@
         <f aca="false">SUM(B16:U16)</f>
         <v>19</v>
       </c>
+      <c r="AG16" s="0" t="n">
+        <f aca="false">SUM(AA16:AE16)</f>
+        <v>9</v>
+      </c>
+      <c r="AH16" s="0" t="n">
+        <f aca="false">SUM(V16:Z16)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -2031,6 +2164,14 @@
         <f aca="false">SUM(B17:U17)</f>
         <v>20</v>
       </c>
+      <c r="AG17" s="0" t="n">
+        <f aca="false">SUM(AA17:AE17)</f>
+        <v>10</v>
+      </c>
+      <c r="AH17" s="0" t="n">
+        <f aca="false">SUM(V17:Z17)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -2140,6 +2281,14 @@
         <f aca="false">SUM(B18:U18)</f>
         <v>19</v>
       </c>
+      <c r="AG18" s="0" t="n">
+        <f aca="false">SUM(AA18:AE18)</f>
+        <v>10</v>
+      </c>
+      <c r="AH18" s="0" t="n">
+        <f aca="false">SUM(V18:Z18)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -2249,6 +2398,14 @@
         <f aca="false">SUM(B19:U19)</f>
         <v>20</v>
       </c>
+      <c r="AG19" s="0" t="n">
+        <f aca="false">SUM(AA19:AE19)</f>
+        <v>10</v>
+      </c>
+      <c r="AH19" s="0" t="n">
+        <f aca="false">SUM(V19:Z19)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -2358,6 +2515,14 @@
         <f aca="false">SUM(B20:U20)</f>
         <v>20</v>
       </c>
+      <c r="AG20" s="0" t="n">
+        <f aca="false">SUM(AA20:AE20)</f>
+        <v>10</v>
+      </c>
+      <c r="AH20" s="0" t="n">
+        <f aca="false">SUM(V20:Z20)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -2467,6 +2632,14 @@
         <f aca="false">SUM(B21:U21)</f>
         <v>20</v>
       </c>
+      <c r="AG21" s="0" t="n">
+        <f aca="false">SUM(AA21:AE21)</f>
+        <v>10</v>
+      </c>
+      <c r="AH21" s="0" t="n">
+        <f aca="false">SUM(V21:Z21)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -2576,6 +2749,14 @@
         <f aca="false">SUM(B22:U22)</f>
         <v>20</v>
       </c>
+      <c r="AG22" s="0" t="n">
+        <f aca="false">SUM(AA22:AE22)</f>
+        <v>10</v>
+      </c>
+      <c r="AH22" s="0" t="n">
+        <f aca="false">SUM(V22:Z22)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -2685,6 +2866,14 @@
         <f aca="false">SUM(B23:U23)</f>
         <v>20</v>
       </c>
+      <c r="AG23" s="0" t="n">
+        <f aca="false">SUM(AA23:AE23)</f>
+        <v>10</v>
+      </c>
+      <c r="AH23" s="0" t="n">
+        <f aca="false">SUM(V23:Z23)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -2794,6 +2983,14 @@
         <f aca="false">SUM(B24:U24)</f>
         <v>19</v>
       </c>
+      <c r="AG24" s="0" t="n">
+        <f aca="false">SUM(AA24:AE24)</f>
+        <v>9</v>
+      </c>
+      <c r="AH24" s="0" t="n">
+        <f aca="false">SUM(V24:Z24)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -2903,6 +3100,14 @@
         <f aca="false">SUM(B25:U25)</f>
         <v>19</v>
       </c>
+      <c r="AG25" s="0" t="n">
+        <f aca="false">SUM(AA25:AE25)</f>
+        <v>9</v>
+      </c>
+      <c r="AH25" s="0" t="n">
+        <f aca="false">SUM(V25:Z25)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -3012,6 +3217,14 @@
         <f aca="false">SUM(B26:U26)</f>
         <v>20</v>
       </c>
+      <c r="AG26" s="0" t="n">
+        <f aca="false">SUM(AA26:AE26)</f>
+        <v>10</v>
+      </c>
+      <c r="AH26" s="0" t="n">
+        <f aca="false">SUM(V26:Z26)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -3121,6 +3334,14 @@
         <f aca="false">SUM(B27:U27)</f>
         <v>20</v>
       </c>
+      <c r="AG27" s="0" t="n">
+        <f aca="false">SUM(AA27:AE27)</f>
+        <v>10</v>
+      </c>
+      <c r="AH27" s="0" t="n">
+        <f aca="false">SUM(V27:Z27)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -3230,6 +3451,14 @@
         <f aca="false">SUM(B28:U28)</f>
         <v>20</v>
       </c>
+      <c r="AG28" s="0" t="n">
+        <f aca="false">SUM(AA28:AE28)</f>
+        <v>10</v>
+      </c>
+      <c r="AH28" s="0" t="n">
+        <f aca="false">SUM(V28:Z28)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -3339,6 +3568,14 @@
         <f aca="false">SUM(B29:U29)</f>
         <v>20</v>
       </c>
+      <c r="AG29" s="0" t="n">
+        <f aca="false">SUM(AA29:AE29)</f>
+        <v>10</v>
+      </c>
+      <c r="AH29" s="0" t="n">
+        <f aca="false">SUM(V29:Z29)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -3448,6 +3685,14 @@
         <f aca="false">SUM(B30:U30)</f>
         <v>20</v>
       </c>
+      <c r="AG30" s="0" t="n">
+        <f aca="false">SUM(AA30:AE30)</f>
+        <v>10</v>
+      </c>
+      <c r="AH30" s="0" t="n">
+        <f aca="false">SUM(V30:Z30)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -3557,6 +3802,14 @@
         <f aca="false">SUM(B31:U31)</f>
         <v>20</v>
       </c>
+      <c r="AG31" s="0" t="n">
+        <f aca="false">SUM(AA31:AE31)</f>
+        <v>10</v>
+      </c>
+      <c r="AH31" s="0" t="n">
+        <f aca="false">SUM(V31:Z31)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -3666,6 +3919,14 @@
         <f aca="false">SUM(B32:U32)</f>
         <v>20</v>
       </c>
+      <c r="AG32" s="0" t="n">
+        <f aca="false">SUM(AA32:AE32)</f>
+        <v>10</v>
+      </c>
+      <c r="AH32" s="0" t="n">
+        <f aca="false">SUM(V32:Z32)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -3775,6 +4036,14 @@
         <f aca="false">SUM(B33:U33)</f>
         <v>17</v>
       </c>
+      <c r="AG33" s="0" t="n">
+        <f aca="false">SUM(AA33:AE33)</f>
+        <v>8</v>
+      </c>
+      <c r="AH33" s="0" t="n">
+        <f aca="false">SUM(V33:Z33)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -3884,6 +4153,14 @@
         <f aca="false">SUM(B34:U34)</f>
         <v>19</v>
       </c>
+      <c r="AG34" s="0" t="n">
+        <f aca="false">SUM(AA34:AE34)</f>
+        <v>9</v>
+      </c>
+      <c r="AH34" s="0" t="n">
+        <f aca="false">SUM(V34:Z34)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -3993,6 +4270,14 @@
         <f aca="false">SUM(B35:U35)</f>
         <v>18</v>
       </c>
+      <c r="AG35" s="0" t="n">
+        <f aca="false">SUM(AA35:AE35)</f>
+        <v>9</v>
+      </c>
+      <c r="AH35" s="0" t="n">
+        <f aca="false">SUM(V35:Z35)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -4102,6 +4387,14 @@
         <f aca="false">SUM(B36:U36)</f>
         <v>18</v>
       </c>
+      <c r="AG36" s="0" t="n">
+        <f aca="false">SUM(AA36:AE36)</f>
+        <v>9</v>
+      </c>
+      <c r="AH36" s="0" t="n">
+        <f aca="false">SUM(V36:Z36)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -4211,6 +4504,14 @@
         <f aca="false">SUM(B37:U37)</f>
         <v>17</v>
       </c>
+      <c r="AG37" s="0" t="n">
+        <f aca="false">SUM(AA37:AE37)</f>
+        <v>9</v>
+      </c>
+      <c r="AH37" s="0" t="n">
+        <f aca="false">SUM(V37:Z37)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
@@ -4320,6 +4621,14 @@
         <f aca="false">SUM(B38:U38)</f>
         <v>18</v>
       </c>
+      <c r="AG38" s="0" t="n">
+        <f aca="false">SUM(AA38:AE38)</f>
+        <v>9</v>
+      </c>
+      <c r="AH38" s="0" t="n">
+        <f aca="false">SUM(V38:Z38)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -4429,6 +4738,14 @@
         <f aca="false">SUM(B39:U39)</f>
         <v>18</v>
       </c>
+      <c r="AG39" s="0" t="n">
+        <f aca="false">SUM(AA39:AE39)</f>
+        <v>9</v>
+      </c>
+      <c r="AH39" s="0" t="n">
+        <f aca="false">SUM(V39:Z39)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -4538,6 +4855,14 @@
         <f aca="false">SUM(B40:U40)</f>
         <v>18</v>
       </c>
+      <c r="AG40" s="0" t="n">
+        <f aca="false">SUM(AA40:AE40)</f>
+        <v>9</v>
+      </c>
+      <c r="AH40" s="0" t="n">
+        <f aca="false">SUM(V40:Z40)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -4647,6 +4972,14 @@
         <f aca="false">SUM(B41:U41)</f>
         <v>15</v>
       </c>
+      <c r="AG41" s="0" t="n">
+        <f aca="false">SUM(AA41:AE41)</f>
+        <v>8</v>
+      </c>
+      <c r="AH41" s="0" t="n">
+        <f aca="false">SUM(V41:Z41)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -4756,6 +5089,14 @@
         <f aca="false">SUM(B42:U42)</f>
         <v>16</v>
       </c>
+      <c r="AG42" s="0" t="n">
+        <f aca="false">SUM(AA42:AE42)</f>
+        <v>9</v>
+      </c>
+      <c r="AH42" s="0" t="n">
+        <f aca="false">SUM(V42:Z42)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -4865,6 +5206,14 @@
         <f aca="false">SUM(B43:U43)</f>
         <v>16</v>
       </c>
+      <c r="AG43" s="0" t="n">
+        <f aca="false">SUM(AA43:AE43)</f>
+        <v>9</v>
+      </c>
+      <c r="AH43" s="0" t="n">
+        <f aca="false">SUM(V43:Z43)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -4974,6 +5323,14 @@
         <f aca="false">SUM(B44:U44)</f>
         <v>16</v>
       </c>
+      <c r="AG44" s="0" t="n">
+        <f aca="false">SUM(AA44:AE44)</f>
+        <v>9</v>
+      </c>
+      <c r="AH44" s="0" t="n">
+        <f aca="false">SUM(V44:Z44)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -5083,6 +5440,14 @@
         <f aca="false">SUM(B45:U45)</f>
         <v>16</v>
       </c>
+      <c r="AG45" s="0" t="n">
+        <f aca="false">SUM(AA45:AE45)</f>
+        <v>9</v>
+      </c>
+      <c r="AH45" s="0" t="n">
+        <f aca="false">SUM(V45:Z45)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -5192,6 +5557,14 @@
         <f aca="false">SUM(B46:U46)</f>
         <v>17</v>
       </c>
+      <c r="AG46" s="0" t="n">
+        <f aca="false">SUM(AA46:AE46)</f>
+        <v>9</v>
+      </c>
+      <c r="AH46" s="0" t="n">
+        <f aca="false">SUM(V46:Z46)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
@@ -5301,6 +5674,14 @@
         <f aca="false">SUM(B47:U47)</f>
         <v>16</v>
       </c>
+      <c r="AG47" s="0" t="n">
+        <f aca="false">SUM(AA47:AE47)</f>
+        <v>9</v>
+      </c>
+      <c r="AH47" s="0" t="n">
+        <f aca="false">SUM(V47:Z47)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -5410,6 +5791,14 @@
         <f aca="false">SUM(B48:U48)</f>
         <v>17</v>
       </c>
+      <c r="AG48" s="0" t="n">
+        <f aca="false">SUM(AA48:AE48)</f>
+        <v>9</v>
+      </c>
+      <c r="AH48" s="0" t="n">
+        <f aca="false">SUM(V48:Z48)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
@@ -5519,6 +5908,14 @@
         <f aca="false">SUM(B49:U49)</f>
         <v>16</v>
       </c>
+      <c r="AG49" s="0" t="n">
+        <f aca="false">SUM(AA49:AE49)</f>
+        <v>9</v>
+      </c>
+      <c r="AH49" s="0" t="n">
+        <f aca="false">SUM(V49:Z49)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
@@ -5628,6 +6025,14 @@
         <f aca="false">SUM(B50:U50)</f>
         <v>16</v>
       </c>
+      <c r="AG50" s="0" t="n">
+        <f aca="false">SUM(AA50:AE50)</f>
+        <v>9</v>
+      </c>
+      <c r="AH50" s="0" t="n">
+        <f aca="false">SUM(V50:Z50)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
@@ -5737,6 +6142,14 @@
         <f aca="false">SUM(B51:U51)</f>
         <v>16</v>
       </c>
+      <c r="AG51" s="0" t="n">
+        <f aca="false">SUM(AA51:AE51)</f>
+        <v>8</v>
+      </c>
+      <c r="AH51" s="0" t="n">
+        <f aca="false">SUM(V51:Z51)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -5846,6 +6259,14 @@
         <f aca="false">SUM(B52:U52)</f>
         <v>17</v>
       </c>
+      <c r="AG52" s="0" t="n">
+        <f aca="false">SUM(AA52:AE52)</f>
+        <v>9</v>
+      </c>
+      <c r="AH52" s="0" t="n">
+        <f aca="false">SUM(V52:Z52)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -5955,6 +6376,14 @@
         <f aca="false">SUM(B53:U53)</f>
         <v>14</v>
       </c>
+      <c r="AG53" s="0" t="n">
+        <f aca="false">SUM(AA53:AE53)</f>
+        <v>8</v>
+      </c>
+      <c r="AH53" s="0" t="n">
+        <f aca="false">SUM(V53:Z53)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
@@ -6064,6 +6493,14 @@
         <f aca="false">SUM(B54:U54)</f>
         <v>14</v>
       </c>
+      <c r="AG54" s="0" t="n">
+        <f aca="false">SUM(AA54:AE54)</f>
+        <v>8</v>
+      </c>
+      <c r="AH54" s="0" t="n">
+        <f aca="false">SUM(V54:Z54)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
@@ -6173,6 +6610,14 @@
         <f aca="false">SUM(B55:U55)</f>
         <v>16</v>
       </c>
+      <c r="AG55" s="0" t="n">
+        <f aca="false">SUM(AA55:AE55)</f>
+        <v>8</v>
+      </c>
+      <c r="AH55" s="0" t="n">
+        <f aca="false">SUM(V55:Z55)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
@@ -6282,6 +6727,14 @@
         <f aca="false">SUM(B56:U56)</f>
         <v>16</v>
       </c>
+      <c r="AG56" s="0" t="n">
+        <f aca="false">SUM(AA56:AE56)</f>
+        <v>8</v>
+      </c>
+      <c r="AH56" s="0" t="n">
+        <f aca="false">SUM(V56:Z56)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
@@ -6391,6 +6844,14 @@
         <f aca="false">SUM(B57:U57)</f>
         <v>15</v>
       </c>
+      <c r="AG57" s="0" t="n">
+        <f aca="false">SUM(AA57:AE57)</f>
+        <v>8</v>
+      </c>
+      <c r="AH57" s="0" t="n">
+        <f aca="false">SUM(V57:Z57)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
@@ -6500,6 +6961,14 @@
         <f aca="false">SUM(B58:U58)</f>
         <v>15</v>
       </c>
+      <c r="AG58" s="0" t="n">
+        <f aca="false">SUM(AA58:AE58)</f>
+        <v>8</v>
+      </c>
+      <c r="AH58" s="0" t="n">
+        <f aca="false">SUM(V58:Z58)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
@@ -6609,6 +7078,14 @@
         <f aca="false">SUM(B59:U59)</f>
         <v>15</v>
       </c>
+      <c r="AG59" s="0" t="n">
+        <f aca="false">SUM(AA59:AE59)</f>
+        <v>8</v>
+      </c>
+      <c r="AH59" s="0" t="n">
+        <f aca="false">SUM(V59:Z59)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
@@ -6718,6 +7195,14 @@
         <f aca="false">SUM(B60:U60)</f>
         <v>15</v>
       </c>
+      <c r="AG60" s="0" t="n">
+        <f aca="false">SUM(AA60:AE60)</f>
+        <v>8</v>
+      </c>
+      <c r="AH60" s="0" t="n">
+        <f aca="false">SUM(V60:Z60)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
@@ -6827,6 +7312,14 @@
         <f aca="false">SUM(B61:U61)</f>
         <v>15</v>
       </c>
+      <c r="AG61" s="0" t="n">
+        <f aca="false">SUM(AA61:AE61)</f>
+        <v>8</v>
+      </c>
+      <c r="AH61" s="0" t="n">
+        <f aca="false">SUM(V61:Z61)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
@@ -6936,6 +7429,14 @@
         <f aca="false">SUM(B62:U62)</f>
         <v>15</v>
       </c>
+      <c r="AG62" s="0" t="n">
+        <f aca="false">SUM(AA62:AE62)</f>
+        <v>8</v>
+      </c>
+      <c r="AH62" s="0" t="n">
+        <f aca="false">SUM(V62:Z62)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
@@ -7045,6 +7546,14 @@
         <f aca="false">SUM(B63:U63)</f>
         <v>14</v>
       </c>
+      <c r="AG63" s="0" t="n">
+        <f aca="false">SUM(AA63:AE63)</f>
+        <v>8</v>
+      </c>
+      <c r="AH63" s="0" t="n">
+        <f aca="false">SUM(V63:Z63)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
@@ -7154,6 +7663,14 @@
         <f aca="false">SUM(B64:U64)</f>
         <v>14</v>
       </c>
+      <c r="AG64" s="0" t="n">
+        <f aca="false">SUM(AA64:AE64)</f>
+        <v>8</v>
+      </c>
+      <c r="AH64" s="0" t="n">
+        <f aca="false">SUM(V64:Z64)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
@@ -7263,6 +7780,14 @@
         <f aca="false">SUM(B65:U65)</f>
         <v>13</v>
       </c>
+      <c r="AG65" s="0" t="n">
+        <f aca="false">SUM(AA65:AE65)</f>
+        <v>7</v>
+      </c>
+      <c r="AH65" s="0" t="n">
+        <f aca="false">SUM(V65:Z65)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
@@ -7372,6 +7897,14 @@
         <f aca="false">SUM(B66:U66)</f>
         <v>15</v>
       </c>
+      <c r="AG66" s="0" t="n">
+        <f aca="false">SUM(AA66:AE66)</f>
+        <v>8</v>
+      </c>
+      <c r="AH66" s="0" t="n">
+        <f aca="false">SUM(V66:Z66)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
@@ -7481,6 +8014,14 @@
         <f aca="false">SUM(B67:U67)</f>
         <v>15</v>
       </c>
+      <c r="AG67" s="0" t="n">
+        <f aca="false">SUM(AA67:AE67)</f>
+        <v>8</v>
+      </c>
+      <c r="AH67" s="0" t="n">
+        <f aca="false">SUM(V67:Z67)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
@@ -7590,6 +8131,14 @@
         <f aca="false">SUM(B68:U68)</f>
         <v>16</v>
       </c>
+      <c r="AG68" s="0" t="n">
+        <f aca="false">SUM(AA68:AE68)</f>
+        <v>9</v>
+      </c>
+      <c r="AH68" s="0" t="n">
+        <f aca="false">SUM(V68:Z68)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
@@ -7699,6 +8248,14 @@
         <f aca="false">SUM(B69:U69)</f>
         <v>16</v>
       </c>
+      <c r="AG69" s="0" t="n">
+        <f aca="false">SUM(AA69:AE69)</f>
+        <v>9</v>
+      </c>
+      <c r="AH69" s="0" t="n">
+        <f aca="false">SUM(V69:Z69)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
@@ -7808,6 +8365,14 @@
         <f aca="false">SUM(B70:U70)</f>
         <v>16</v>
       </c>
+      <c r="AG70" s="0" t="n">
+        <f aca="false">SUM(AA70:AE70)</f>
+        <v>9</v>
+      </c>
+      <c r="AH70" s="0" t="n">
+        <f aca="false">SUM(V70:Z70)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
@@ -7917,6 +8482,14 @@
         <f aca="false">SUM(B71:U71)</f>
         <v>16</v>
       </c>
+      <c r="AG71" s="0" t="n">
+        <f aca="false">SUM(AA71:AE71)</f>
+        <v>9</v>
+      </c>
+      <c r="AH71" s="0" t="n">
+        <f aca="false">SUM(V71:Z71)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
@@ -8025,6 +8598,14 @@
       <c r="AF72" s="3" t="n">
         <f aca="false">SUM(B72:U72)</f>
         <v>16</v>
+      </c>
+      <c r="AG72" s="0" t="n">
+        <f aca="false">SUM(AA72:AE72)</f>
+        <v>9</v>
+      </c>
+      <c r="AH72" s="0" t="n">
+        <f aca="false">SUM(V72:Z72)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>